<commit_message>
Wrapping up for this work session
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="0" windowWidth="13460" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="11340" yWindow="0" windowWidth="13460" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offramp coordinates.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
   <si>
     <t>Imperial Highway west</t>
   </si>
@@ -454,12 +454,6 @@
   </si>
   <si>
     <t>maybe redo these</t>
-  </si>
-  <si>
-    <t>// subtract one from all of these</t>
-  </si>
-  <si>
-    <t>// subtract 1?</t>
   </si>
   <si>
     <t>Index</t>
@@ -523,8 +517,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -589,7 +585,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -617,6 +613,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -644,6 +641,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3290,8 +3288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3307,9 +3305,6 @@
       <c r="A1" s="1">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="C2" s="1" t="s">
@@ -3616,11 +3611,6 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="E28" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>10</v>
@@ -4164,8 +4154,8 @@
       <c r="D71" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>145</v>
+      <c r="E71" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -5037,7 +5027,7 @@
         <v>139</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -5049,6 +5039,9 @@
       </c>
       <c r="D132" s="1">
         <v>-118.369896</v>
+      </c>
+      <c r="E132" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:5">

</xml_diff>

<commit_message>
Done with those coordinates
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13460" yWindow="0" windowWidth="12120" windowHeight="14140" tabRatio="500"/>
+    <workbookView xWindow="14200" yWindow="0" windowWidth="20560" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offramp coordinates.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="147">
   <si>
     <t>Imperial Highway west</t>
   </si>
@@ -441,18 +441,9 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Eastbound</t>
-  </si>
-  <si>
     <t>Index of matching point</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>maybe redo these</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -460,6 +451,15 @@
   </si>
   <si>
     <t>Made this one</t>
+  </si>
+  <si>
+    <t>decreased</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>dec</t>
   </si>
 </sst>
 </file>
@@ -520,8 +520,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -592,7 +614,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -623,6 +645,17 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +686,17 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3299,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3312,12 +3356,12 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
@@ -3325,10 +3369,10 @@
         <v>139</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3342,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3353,10 +3397,10 @@
         <v>-118.396164</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3367,10 +3411,10 @@
         <v>-118.387473</v>
       </c>
       <c r="E5" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3381,10 +3425,10 @@
         <v>-118.370007</v>
       </c>
       <c r="E6" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -3395,10 +3439,10 @@
         <v>-118.368419</v>
       </c>
       <c r="E7" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3409,10 +3453,13 @@
         <v>-118.352605</v>
       </c>
       <c r="E8" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -3423,10 +3470,10 @@
         <v>-118.34385</v>
       </c>
       <c r="E9" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3437,10 +3484,10 @@
         <v>-118.32658000000001</v>
       </c>
       <c r="E10" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3451,10 +3498,10 @@
         <v>-118.29173299999999</v>
       </c>
       <c r="E11" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -3465,10 +3512,10 @@
         <v>-118.28066</v>
       </c>
       <c r="E12" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -3479,10 +3526,10 @@
         <v>-118.254329</v>
       </c>
       <c r="E13" s="1">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -3493,10 +3540,10 @@
         <v>-118.209976</v>
       </c>
       <c r="E14" s="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3507,10 +3554,10 @@
         <v>-118.209976</v>
       </c>
       <c r="E15" s="1">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -3521,10 +3568,10 @@
         <v>-118.180042</v>
       </c>
       <c r="E16" s="1">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3535,10 +3582,10 @@
         <v>-118.168927</v>
       </c>
       <c r="E17" s="1">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3549,10 +3596,10 @@
         <v>-118.159936</v>
       </c>
       <c r="E18" s="1">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3563,10 +3610,10 @@
         <v>-118.140428</v>
       </c>
       <c r="E19" s="1">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3577,10 +3624,10 @@
         <v>-118.12542000000001</v>
       </c>
       <c r="E20" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -3591,10 +3638,10 @@
         <v>-118.104692</v>
       </c>
       <c r="E21" s="1">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3605,10 +3652,10 @@
         <v>-118.10342</v>
       </c>
       <c r="E22" s="1">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3619,10 +3666,10 @@
         <v>-118.099153</v>
       </c>
       <c r="E23" s="1">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>10</v>
       </c>
@@ -3633,10 +3680,10 @@
         <v>139</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3647,10 +3694,13 @@
         <v>-118.49547</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>336</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -3661,10 +3711,10 @@
         <v>-118.48933</v>
       </c>
       <c r="E31" s="1">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -3675,10 +3725,10 @@
         <v>-118.485857</v>
       </c>
       <c r="E32" s="1">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
@@ -3689,10 +3739,10 @@
         <v>-118.473798</v>
       </c>
       <c r="E33" s="1">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -3703,10 +3753,10 @@
         <v>-118.469356</v>
       </c>
       <c r="E34" s="1">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -3717,10 +3767,10 @@
         <v>-118.455172</v>
       </c>
       <c r="E35" s="1">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
         <v>27</v>
       </c>
@@ -3731,10 +3781,10 @@
         <v>-118.44925000000001</v>
       </c>
       <c r="E36" s="1">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>28</v>
       </c>
@@ -3745,10 +3795,10 @@
         <v>-118.43358600000001</v>
       </c>
       <c r="E37" s="1">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>29</v>
       </c>
@@ -3759,10 +3809,10 @@
         <v>-118.41702100000001</v>
       </c>
       <c r="E38" s="1">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
@@ -3773,10 +3823,10 @@
         <v>-118.40318000000001</v>
       </c>
       <c r="E39" s="1">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
@@ -3787,10 +3837,10 @@
         <v>-118.391379</v>
       </c>
       <c r="E40" s="1">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
@@ -3801,10 +3851,10 @@
         <v>-118.377431</v>
       </c>
       <c r="E41" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
@@ -3815,10 +3865,10 @@
         <v>-118.369535</v>
       </c>
       <c r="E42" s="1">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
@@ -3829,10 +3879,10 @@
         <v>-118.350137</v>
       </c>
       <c r="E43" s="1">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
@@ -3843,10 +3893,10 @@
         <v>-118.333786</v>
       </c>
       <c r="E44" s="1">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
@@ -3857,10 +3907,13 @@
         <v>-118.31771500000001</v>
       </c>
       <c r="E45" s="1">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>192</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="6" t="s">
         <v>36</v>
       </c>
@@ -3872,10 +3925,10 @@
         <v>-118.30052999999999</v>
       </c>
       <c r="E46" s="1">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
@@ -3886,10 +3939,10 @@
         <v>-118.291601</v>
       </c>
       <c r="E47" s="1">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
@@ -3900,7 +3953,7 @@
         <v>-118.28396499999999</v>
       </c>
       <c r="E48" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3914,7 +3967,7 @@
         <v>-118.273966</v>
       </c>
       <c r="E49" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3928,7 +3981,7 @@
         <v>-118.267117</v>
       </c>
       <c r="E50" s="1">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3942,7 +3995,7 @@
         <v>-118.26239700000001</v>
       </c>
       <c r="E51" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3956,7 +4009,7 @@
         <v>-118.259972</v>
       </c>
       <c r="E52" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3970,7 +4023,7 @@
         <v>-118.256174</v>
       </c>
       <c r="E53" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3984,7 +4037,7 @@
         <v>-118.249222</v>
       </c>
       <c r="E54" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3998,7 +4051,7 @@
         <v>-118.239287</v>
       </c>
       <c r="E55" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -4012,7 +4065,7 @@
         <v>-118.231111</v>
       </c>
       <c r="E56" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -4026,7 +4079,7 @@
         <v>-118.224653</v>
       </c>
       <c r="E57" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -4040,7 +4093,7 @@
         <v>-118.220799</v>
       </c>
       <c r="E58" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -4054,7 +4107,7 @@
         <v>-118.217259</v>
       </c>
       <c r="E59" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -4068,7 +4121,7 @@
         <v>-118.21423299999999</v>
       </c>
       <c r="E60" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4082,7 +4135,7 @@
         <v>-118.21405300000001</v>
       </c>
       <c r="E61" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4096,7 +4149,7 @@
         <v>-118.213751</v>
       </c>
       <c r="E62" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -4110,7 +4163,7 @@
         <v>-118.211658</v>
       </c>
       <c r="E63" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -4124,7 +4177,7 @@
         <v>-118.200599</v>
       </c>
       <c r="E64" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -4138,7 +4191,7 @@
         <v>-118.186156</v>
       </c>
       <c r="E65" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -4155,6 +4208,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70" spans="1:5">
+      <c r="E70" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>101</v>
@@ -4166,7 +4224,7 @@
         <v>139</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4180,7 +4238,7 @@
         <v>-118.20836300000001</v>
       </c>
       <c r="E72" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -4194,7 +4252,7 @@
         <v>-118.209715</v>
       </c>
       <c r="E73" s="1">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -4208,7 +4266,7 @@
         <v>-118.214382</v>
       </c>
       <c r="E74" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4222,7 +4280,7 @@
         <v>-118.221254</v>
       </c>
       <c r="E75" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4236,7 +4294,7 @@
         <v>-118.22113</v>
       </c>
       <c r="E76" s="1">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4250,7 +4308,7 @@
         <v>-118.22141999999999</v>
       </c>
       <c r="E77" s="1">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4264,7 +4322,7 @@
         <v>-118.224006</v>
       </c>
       <c r="E78" s="1">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4278,7 +4336,7 @@
         <v>-118.225594</v>
       </c>
       <c r="E79" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -4292,10 +4350,10 @@
         <v>-118.22671099999999</v>
       </c>
       <c r="E80" s="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>63</v>
       </c>
@@ -4306,10 +4364,10 @@
         <v>-118.232449</v>
       </c>
       <c r="E81" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>64</v>
       </c>
@@ -4320,10 +4378,10 @@
         <v>-118.2379</v>
       </c>
       <c r="E82" s="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>65</v>
       </c>
@@ -4334,10 +4392,10 @@
         <v>-118.23931899999999</v>
       </c>
       <c r="E83" s="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>66</v>
       </c>
@@ -4348,10 +4406,10 @@
         <v>-118.241354</v>
       </c>
       <c r="E84" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="2" t="s">
         <v>67</v>
       </c>
@@ -4362,10 +4420,10 @@
         <v>-118.242379</v>
       </c>
       <c r="E85" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="2" t="s">
         <v>68</v>
       </c>
@@ -4376,10 +4434,10 @@
         <v>-118.24545000000001</v>
       </c>
       <c r="E86" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="2" t="s">
         <v>69</v>
       </c>
@@ -4390,10 +4448,10 @@
         <v>-118.24871400000001</v>
       </c>
       <c r="E87" s="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="2" t="s">
         <v>70</v>
       </c>
@@ -4404,10 +4462,10 @@
         <v>-118.260645</v>
       </c>
       <c r="E88" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="2" t="s">
         <v>71</v>
       </c>
@@ -4418,10 +4476,10 @@
         <v>-118.266937</v>
       </c>
       <c r="E89" s="1">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="2" t="s">
         <v>72</v>
       </c>
@@ -4432,10 +4490,10 @@
         <v>-118.273117</v>
       </c>
       <c r="E90" s="1">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="2" t="s">
         <v>73</v>
       </c>
@@ -4446,10 +4504,10 @@
         <v>-118.281485</v>
       </c>
       <c r="E91" s="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -4460,13 +4518,10 @@
         <v>-118.29159300000001</v>
       </c>
       <c r="E92" s="1">
-        <v>114</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="2" t="s">
         <v>74</v>
       </c>
@@ -4477,10 +4532,10 @@
         <v>-118.298315</v>
       </c>
       <c r="E93" s="1">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="2" t="s">
         <v>75</v>
       </c>
@@ -4491,10 +4546,10 @@
         <v>-118.305577</v>
       </c>
       <c r="E94" s="1">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="2" t="s">
         <v>76</v>
       </c>
@@ -4505,10 +4560,10 @@
         <v>-118.314562</v>
       </c>
       <c r="E95" s="1">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="2" t="s">
         <v>77</v>
       </c>
@@ -4519,7 +4574,7 @@
         <v>-118.316762</v>
       </c>
       <c r="E96" s="1">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -4533,7 +4588,7 @@
         <v>-118.322408</v>
       </c>
       <c r="E97" s="1">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4547,7 +4602,7 @@
         <v>-118.32666999999999</v>
       </c>
       <c r="E98" s="1">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4561,7 +4616,7 @@
         <v>-118.33067200000001</v>
       </c>
       <c r="E99" s="1">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4575,7 +4630,7 @@
         <v>-118.33525299999999</v>
       </c>
       <c r="E100" s="1">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4589,7 +4644,7 @@
         <v>-118.34840699999999</v>
       </c>
       <c r="E101" s="1">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4603,7 +4658,7 @@
         <v>-118.352368</v>
       </c>
       <c r="E102" s="1">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4617,7 +4672,7 @@
         <v>-118.362826</v>
       </c>
       <c r="E103" s="1">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4631,7 +4686,7 @@
         <v>-118.364811</v>
       </c>
       <c r="E104" s="1">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4645,7 +4700,7 @@
         <v>-118.37136599999999</v>
       </c>
       <c r="E105" s="1">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4659,7 +4714,7 @@
         <v>-118.37696800000001</v>
       </c>
       <c r="E106" s="1">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4673,7 +4728,7 @@
         <v>-118.375069</v>
       </c>
       <c r="E107" s="1">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4687,7 +4742,7 @@
         <v>-118.37935899999999</v>
       </c>
       <c r="E108" s="1">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4701,7 +4756,7 @@
         <v>-118.396343</v>
       </c>
       <c r="E109" s="1">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4715,10 +4770,10 @@
         <v>-118.41387899999999</v>
       </c>
       <c r="E110" s="1">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4732,10 +4787,7 @@
         <v>-118.43136699999999</v>
       </c>
       <c r="E111" s="1">
-        <v>217</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>142</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4749,10 +4801,7 @@
         <v>-118.448807</v>
       </c>
       <c r="E112" s="1">
-        <v>228</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>143</v>
+        <v>226</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4766,10 +4815,7 @@
         <v>-118.46623099999999</v>
       </c>
       <c r="E113" s="1">
-        <v>237</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>143</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4783,10 +4829,7 @@
         <v>-118.469964</v>
       </c>
       <c r="E114" s="1">
-        <v>245</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>143</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4800,10 +4843,7 @@
         <v>-118.47398800000001</v>
       </c>
       <c r="E115" s="1">
-        <v>254</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>143</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -4817,10 +4857,7 @@
         <v>-118.492205</v>
       </c>
       <c r="E116" s="1">
-        <v>258</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -4834,10 +4871,7 @@
         <v>-118.501335</v>
       </c>
       <c r="E117" s="1">
-        <v>266</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>143</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -4851,10 +4885,7 @@
         <v>-118.51880199999999</v>
       </c>
       <c r="E118" s="1">
-        <v>273</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>143</v>
+        <v>272</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -4868,10 +4899,7 @@
         <v>-118.53628999999999</v>
       </c>
       <c r="E119" s="1">
-        <v>283</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>143</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4885,7 +4913,7 @@
         <v>-118.553681</v>
       </c>
       <c r="E120" s="1">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>143</v>
@@ -4904,9 +4932,6 @@
       <c r="E121" s="1">
         <v>292</v>
       </c>
-      <c r="F121" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="2" t="s">
@@ -4921,9 +4946,6 @@
       <c r="E122" s="1">
         <v>300</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="2" t="s">
@@ -4938,9 +4960,6 @@
       <c r="E123" s="1">
         <v>302</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="2" t="s">
@@ -4953,10 +4972,7 @@
         <v>-118.60601699999999</v>
       </c>
       <c r="E124" s="1">
-        <v>303</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>143</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4972,9 +4988,6 @@
       <c r="E125" s="1">
         <v>311</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" s="2" t="s">
@@ -4987,7 +5000,7 @@
         <v>-118.62613899999999</v>
       </c>
       <c r="E126" s="1">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -5001,10 +5014,10 @@
         <v>-118.630285</v>
       </c>
       <c r="E127" s="1">
-        <v>323</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>146</v>
+        <v>321</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -5018,12 +5031,12 @@
         <v>-118.637012</v>
       </c>
       <c r="E128" s="1">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="E130" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -5037,7 +5050,7 @@
         <v>139</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="132" spans="1:5">

</xml_diff>

<commit_message>
Cars move along path
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14200" yWindow="0" windowWidth="20560" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="17320" yWindow="0" windowWidth="18200" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offramp coordinates.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="155">
   <si>
     <t>Imperial Highway west</t>
   </si>
@@ -460,6 +460,30 @@
   </si>
   <si>
     <t>dec</t>
+  </si>
+  <si>
+    <t>goes left to right, slightly down?</t>
+  </si>
+  <si>
+    <t>Left (west) most</t>
+  </si>
+  <si>
+    <t>Right (east) most</t>
+  </si>
+  <si>
+    <t>Goes right, slightly up, but also down at times</t>
+  </si>
+  <si>
+    <t>goes left, up slightly</t>
+  </si>
+  <si>
+    <t>Down (south)</t>
+  </si>
+  <si>
+    <t>goes up and to the left</t>
+  </si>
+  <si>
+    <t>Up (north most)</t>
   </si>
 </sst>
 </file>
@@ -520,8 +544,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -614,7 +666,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -656,6 +708,20 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -697,6 +763,20 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3341,10 +3421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3356,12 +3436,12 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
@@ -3372,7 +3452,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3385,8 +3465,11 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3399,8 +3482,11 @@
       <c r="E4" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3414,7 +3500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3428,7 +3514,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -3442,7 +3528,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3459,7 +3545,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -3473,7 +3559,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3487,7 +3573,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3501,7 +3587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -3515,7 +3601,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -3529,7 +3615,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -3543,7 +3629,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3557,7 +3643,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -3571,7 +3657,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3585,7 +3671,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3599,7 +3685,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3613,7 +3699,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3627,7 +3713,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -3641,7 +3727,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3655,7 +3741,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3668,8 +3754,11 @@
       <c r="E23" s="1">
         <v>215</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G23" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>10</v>
       </c>
@@ -3683,7 +3772,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3699,8 +3788,11 @@
       <c r="F30" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -3713,8 +3805,11 @@
       <c r="E31" s="1">
         <v>314</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -4180,7 +4275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:7">
       <c r="A65" s="2" t="s">
         <v>54</v>
       </c>
@@ -4194,7 +4289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:7">
       <c r="A66" s="2" t="s">
         <v>55</v>
       </c>
@@ -4207,13 +4302,16 @@
       <c r="E66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="G66" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="E70" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
         <v>101</v>
       </c>
@@ -4227,7 +4325,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:7">
       <c r="A72" s="2" t="s">
         <v>56</v>
       </c>
@@ -4240,8 +4338,11 @@
       <c r="E72" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="G72" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
@@ -4254,8 +4355,11 @@
       <c r="E73" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="G73" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
         <v>58</v>
       </c>
@@ -4269,7 +4373,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:7">
       <c r="A75" s="2" t="s">
         <v>59</v>
       </c>
@@ -4283,7 +4387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
         <v>48</v>
       </c>
@@ -4297,7 +4401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:7">
       <c r="A77" s="2" t="s">
         <v>60</v>
       </c>
@@ -4311,7 +4415,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:7">
       <c r="A78" s="2" t="s">
         <v>49</v>
       </c>
@@ -4325,7 +4429,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:7">
       <c r="A79" s="2" t="s">
         <v>61</v>
       </c>
@@ -4339,7 +4443,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:7">
       <c r="A80" s="2" t="s">
         <v>62</v>
       </c>
@@ -4804,7 +4908,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
         <v>94</v>
       </c>
@@ -4818,7 +4922,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:7">
       <c r="A114" s="2" t="s">
         <v>95</v>
       </c>
@@ -4832,7 +4936,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:7">
       <c r="A115" s="2" t="s">
         <v>96</v>
       </c>
@@ -4846,7 +4950,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:7">
       <c r="A116" s="2" t="s">
         <v>97</v>
       </c>
@@ -4860,7 +4964,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:7">
       <c r="A117" s="2" t="s">
         <v>98</v>
       </c>
@@ -4874,7 +4978,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:7">
       <c r="A118" s="2" t="s">
         <v>99</v>
       </c>
@@ -4888,7 +4992,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:7">
       <c r="A119" s="2" t="s">
         <v>100</v>
       </c>
@@ -4902,7 +5006,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:7">
       <c r="A120" s="2" t="s">
         <v>101</v>
       </c>
@@ -4919,7 +5023,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:7">
       <c r="A121" s="2" t="s">
         <v>102</v>
       </c>
@@ -4933,7 +5037,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:7">
       <c r="A122" s="2" t="s">
         <v>103</v>
       </c>
@@ -4947,7 +5051,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:7">
       <c r="A123" s="2" t="s">
         <v>104</v>
       </c>
@@ -4961,7 +5065,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:7">
       <c r="A124" s="2" t="s">
         <v>105</v>
       </c>
@@ -4975,7 +5079,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:7">
       <c r="A125" s="2" t="s">
         <v>106</v>
       </c>
@@ -4989,7 +5093,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:7">
       <c r="A126" s="2" t="s">
         <v>107</v>
       </c>
@@ -5003,7 +5107,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:7">
       <c r="A127" s="2" t="s">
         <v>108</v>
       </c>
@@ -5020,7 +5124,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:7">
       <c r="A128" s="2" t="s">
         <v>109</v>
       </c>
@@ -5033,13 +5137,16 @@
       <c r="E128" s="1">
         <v>327</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="G128" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="E130" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:6">
       <c r="A131" s="1">
         <v>405</v>
       </c>
@@ -5053,7 +5160,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:6">
       <c r="A132" s="2" t="s">
         <v>110</v>
       </c>
@@ -5066,8 +5173,11 @@
       <c r="E132" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="2" t="s">
         <v>111</v>
       </c>
@@ -5080,8 +5190,11 @@
       <c r="E133" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="2" t="s">
         <v>112</v>
       </c>
@@ -5095,7 +5208,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:6">
       <c r="A135" s="2" t="s">
         <v>113</v>
       </c>
@@ -5109,7 +5222,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:6">
       <c r="A136" s="2" t="s">
         <v>114</v>
       </c>
@@ -5123,7 +5236,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:6">
       <c r="A137" s="2" t="s">
         <v>115</v>
       </c>
@@ -5137,7 +5250,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:6">
       <c r="A138" s="2" t="s">
         <v>116</v>
       </c>
@@ -5151,7 +5264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:6">
       <c r="A139" s="2" t="s">
         <v>117</v>
       </c>
@@ -5165,7 +5278,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:6">
       <c r="A140" s="2" t="s">
         <v>30</v>
       </c>
@@ -5179,7 +5292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:6">
       <c r="A141" s="2" t="s">
         <v>118</v>
       </c>
@@ -5193,7 +5306,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:6">
       <c r="A142" s="2" t="s">
         <v>119</v>
       </c>
@@ -5207,7 +5320,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
         <v>120</v>
       </c>
@@ -5221,7 +5334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:6">
       <c r="A144" s="2" t="s">
         <v>121</v>
       </c>
@@ -5459,7 +5572,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:6">
       <c r="A161" s="2" t="s">
         <v>137</v>
       </c>
@@ -5471,6 +5584,9 @@
       </c>
       <c r="E161" s="1">
         <v>313</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Animates cars from point to point
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17320" yWindow="0" windowWidth="18200" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="18640" yWindow="0" windowWidth="13720" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offramp coordinates.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="162">
   <si>
     <t>Imperial Highway west</t>
   </si>
@@ -484,6 +484,27 @@
   </si>
   <si>
     <t>Up (north most)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -544,8 +565,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,7 +697,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -722,6 +753,11 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -777,6 +813,11 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3421,10 +3462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3436,12 +3477,12 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
@@ -3452,7 +3493,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -3468,8 +3509,11 @@
       <c r="G3" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="K3" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3485,8 +3529,17 @@
       <c r="G4" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="K4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3499,8 +3552,14 @@
       <c r="E5" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="K5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3513,8 +3572,17 @@
       <c r="E6" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="K6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -3527,8 +3595,14 @@
       <c r="E7" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="K7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3545,7 +3619,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -3558,8 +3632,11 @@
       <c r="E9" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="K9" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3572,8 +3649,17 @@
       <c r="E10" s="1">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="K10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3586,8 +3672,14 @@
       <c r="E11" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="K11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -3600,8 +3692,17 @@
       <c r="E12" s="1">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="K12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -3614,8 +3715,14 @@
       <c r="E13" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="K13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -3629,7 +3736,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:13">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -3642,8 +3749,11 @@
       <c r="E15" s="1">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="K15" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -3656,8 +3766,17 @@
       <c r="E16" s="1">
         <v>166</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="K16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -3670,8 +3789,14 @@
       <c r="E17" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="K17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3684,8 +3809,17 @@
       <c r="E18" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="K18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -3698,8 +3832,14 @@
       <c r="E19" s="1">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="K19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3713,7 +3853,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -3726,8 +3866,11 @@
       <c r="E21" s="1">
         <v>205</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="K21" s="1">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3740,8 +3883,14 @@
       <c r="E22" s="1">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="K22" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3757,8 +3906,36 @@
       <c r="G23" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="K23" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="K24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="K25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="1">
         <v>10</v>
       </c>
@@ -3772,7 +3949,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3792,7 +3969,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -3809,7 +3986,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Coordinate update I think
</commit_message>
<xml_diff>
--- a/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
+++ b/Assets/Offramp Coordinate Info/Offramp coordinates with Coordinate indices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18640" yWindow="0" windowWidth="13720" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="18280" yWindow="0" windowWidth="13720" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Offramp coordinates.csv" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -547,6 +547,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -688,7 +694,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,6 +702,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3464,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3529,13 +3536,13 @@
       <c r="G4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3556,7 +3563,7 @@
         <v>156</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3572,13 +3579,13 @@
       <c r="E6" s="1">
         <v>27</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3599,7 +3606,7 @@
         <v>158</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3649,13 +3656,13 @@
       <c r="E10" s="1">
         <v>67</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3692,13 +3699,13 @@
       <c r="E12" s="1">
         <v>91</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3766,13 +3773,13 @@
       <c r="E16" s="1">
         <v>166</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3809,13 +3816,13 @@
       <c r="E18" s="1">
         <v>190</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3906,13 +3913,13 @@
       <c r="G23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L23" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3925,13 +3932,13 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L25" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="7" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>